<commit_message>
Committing files after merging master
</commit_message>
<xml_diff>
--- a/BenadrylAutomation/src/test/resources/TestData/FooterPageTestData.xlsx
+++ b/BenadrylAutomation/src/test/resources/TestData/FooterPageTestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SJI-GOA-70\git\BenadrylAutomation\BenadrylAutomation\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SJI-GOA-69\git\BenadrylAutomation\BenadrylAutomation\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{146171A8-9406-45C3-AC13-2BF82A8E664E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66DB777-0091-4A09-AA42-2585E6F67BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3504" yWindow="1140" windowWidth="20748" windowHeight="9048" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="footer" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>testcase</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Verify the footer link - 'Legal'</t>
+  </si>
+  <si>
+    <t>expected Url</t>
   </si>
 </sst>
 </file>
@@ -513,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,7 +538,7 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -631,9 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE4F141E-2962-415D-80C5-86511ED1A3D3}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -721,9 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D018596-92A4-485D-B2E3-03FD20F36D2E}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -812,9 +811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B90B47-56F5-49EF-B98E-6C288CA10D4F}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>